<commit_message>
Changed flag values to list of integers to see if it satisfies CF compliance checker
</commit_message>
<xml_diff>
--- a/specific_variables/skin-temperature.xlsx
+++ b/specific_variables/skin-temperature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/heather/Desktop/ace-ceda-master/specific_variables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDBC74F-EC77-3E48-AE6B-1258873D6483}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF76E5F1-4AB4-9041-929D-6DF61F655B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5940" yWindow="460" windowWidth="20780" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,10 +94,10 @@
     <t>Surface brightness temperature (9.6-11.5 um)</t>
   </si>
   <si>
-    <t>0b, 1b, 2b, 3b</t>
+    <t>no_data good_data suspect_data_detailed_in_log bad_data_temperature_outside_sensor_operational_range</t>
   </si>
   <si>
-    <t>no_data good_data suspect_data_detailed_in_log bad_data_temperature_outside_sensor_operational_range</t>
+    <t>0, 1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -548,7 +548,7 @@
   <dimension ref="A1:C979"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -692,7 +692,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">
@@ -701,7 +701,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>